<commit_message>
REST API 구현 연습
</commit_message>
<xml_diff>
--- a/(수정)인터페이스명세서_박영근.xlsx
+++ b/(수정)인터페이스명세서_박영근.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\박영근2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6795" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6795" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="인터페이스 목록" sheetId="1" r:id="rId1"/>
@@ -17,13 +12,14 @@
     <sheet name="인터페이스 명세서2" sheetId="5" r:id="rId3"/>
     <sheet name="인터페이스 명세서3" sheetId="3" r:id="rId4"/>
     <sheet name="인터페이스 명세서4" sheetId="4" r:id="rId5"/>
+    <sheet name="인터페이스 명세서5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="101">
   <si>
     <t>구분</t>
   </si>
@@ -98,22 +94,6 @@
   </si>
   <si>
     <t>비고</t>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>pi/board/write</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -136,10 +116,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>BOARD-WEB-003</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자명</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -157,100 +133,6 @@
   </si>
   <si>
     <t>content</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>String</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>error</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>.subject(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>예시)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">필수입력사항(subject) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>에러메세지</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">필수입력사항(content) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>에러메세지</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>error.content(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>예시)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>poster</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -288,14 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>작성자명</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardNo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글번호</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -364,21 +238,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  "boardNo" : 1
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELETE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글 조회(접근권한 : 없음)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>boardNo</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -398,24 +258,91 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>게시글 삭제(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 조회(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/delete/{게시글번호}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/get/{게시글번호}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 목록(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/update/{게시글번호}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 수정(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOARD-WEB-003</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOARD-WEB-001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>errorMessage(예시)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러메세지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/write</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET / application/json</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 목록(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>{
   "subject" :＂글제목",
-  "content" : "글내용",
+  "content" : "글내용"
 }</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>errorMessage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러메시지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>성공시(200)
-{
-  "boardNo" : 1,
-  "poster" : "user01",
-  "subject" : "글제목",
-  "content" : "글내용"
-}
-실패시(400)
-{ 
-  "errorMessage" : "게시글이 존재하지 않습니다</t>
+      <t>s</t>
     </r>
     <r>
       <rPr>
@@ -425,7 +352,61 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>."</t>
+      <t>tring</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOARD-WEB-004</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공시(201)
+응답 데이터 없음
+실패시(400)
+{
+  "status" : "Bad_Request", 
+  "errorMessage" : "삭제에 실패했습니다."
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공시(201)
+응답 데이터 없음
+실패시(400)
+{ 
+  "status" : "Bad_Request",
+  "errorMessage" : "게시글 등록에 실패했습니다."
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOARD-WEB-005</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 수정(접근권한 : 없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/get/{게시글번호}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>응답상태메시지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
     </r>
     <r>
       <rPr>
@@ -435,9 +416,111 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">
+      <t>tring</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오류일경우</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>regDt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modDt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 제목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 내용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>ocalDateTime</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조회 성공일 경우</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공시(200)
+{
+  {
+    "regDt": "2023-06-07T20:57:33.267995",
+    "modDt": null,
+    "id": 202,
+    "subject": "글 제목",
+    "content": "글 내용"
+  },
+  {
+    "regDt": "2023-06-07T20:50:47.511417",
+    "modDt": null,
+    "id": 152,
+    "subject": "글 제목",
+    "content": "글 내용"
+  }
+}
+실패시(400)
+{
+  "status" : "Bad_Request", 
+  "errorMessage" : "조회에 실패했습니다."
 }</t>
-    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "id" : 1
+}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -445,95 +528,43 @@
 응답 데이터 없음
 실패시(400)
 { 
-  "errorMessage" : "이미 존재하는 아이디 입니다."
+  "errorMessage" : "수정에 실패했습니다."
 }</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 삭제(접근권한 : 없음)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 조회(접근권한 : 없음)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/board/delete/{게시글번호}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/board/list</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/board/get/{게시글번호}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 목록(접근권한 : 없음)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/board/update/{게시글번호}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 수정(접근권한 : 없음)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOARD-WEB-003</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOARD-WEB-001</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>api/board/get/{게시글번호}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>api/board/delete/{게시글번호}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>성공시(200)
-응답 데이터 없음
-실패시(400)
-{ 
-  "error.subject" : "글제목을 입력하세요."
-  "error.content" : "글내용을 입력하세요."
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>성공시(201)
-응답 데이터 없음
+{
+    "regDt": "2023-06-07T20:57:33.267995",
+    "modDt": null,
+    "id": 202,
+    "subject": "글 제목",
+    "content": "글 내용"
+}
 실패시(400)
 { 
   "status" : "Bad_Request",
-  "errorMessage" : "게시글 등록에 실패했습니다.",
+  "errorMessage" : "게시글 조회에 실패했습니다.."
 }</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>errorMessage(예시)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>에러메세지</t>
+    <t>조회 성공 시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/delete/{게시글번호}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/board/update/{게시글번호}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1285,7 +1316,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1308,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -1325,22 +1356,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1350,16 +1381,16 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1369,16 +1400,16 @@
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -1388,16 +1419,16 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -1407,16 +1438,16 @@
       <c r="B6" s="19"/>
       <c r="C6" s="18"/>
       <c r="D6" s="5" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -1525,8 +1556,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:F20"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1543,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1555,13 +1586,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -1571,7 +1602,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1608,10 +1639,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -1626,13 +1657,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
@@ -1660,7 +1691,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -1697,28 +1728,40 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="4">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
@@ -1757,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -1782,7 +1825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:F20"/>
     </sheetView>
   </sheetViews>
@@ -1800,7 +1843,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1812,13 +1855,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -1828,7 +1871,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1861,39 +1904,19 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1916,9 +1939,7 @@
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>61</v>
-      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -1954,16 +1975,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
@@ -1974,59 +1995,107 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
+        <v>85</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="4">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="4">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="4">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="126.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -2051,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2069,7 +2138,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2087,7 +2156,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2097,7 +2166,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2130,21 +2199,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2175,9 +2234,7 @@
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>56</v>
-      </c>
+      <c r="B10" s="26"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -2216,13 +2273,13 @@
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
@@ -2233,19 +2290,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2253,19 +2310,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2273,40 +2330,28 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
@@ -2321,7 +2366,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -2346,8 +2391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2364,7 +2409,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2376,13 +2421,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2392,7 +2437,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2429,13 +2474,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
@@ -2471,7 +2516,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -2517,7 +2562,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
@@ -2568,7 +2613,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -2587,4 +2632,239 @@
   <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B20:F20"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
0608 rest api 연습완성본
</commit_message>
<xml_diff>
--- a/(수정)인터페이스명세서_박영근.xlsx
+++ b/(수정)인터페이스명세서_박영근.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PYG\save\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6795" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6795" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="인터페이스 목록" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="102">
   <si>
     <t>구분</t>
   </si>
@@ -170,10 +175,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글번호</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>L</t>
     </r>
@@ -358,16 +359,6 @@
   </si>
   <si>
     <t>BOARD-WEB-004</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>성공시(201)
-응답 데이터 없음
-실패시(400)
-{
-  "status" : "Bad_Request", 
-  "errorMessage" : "삭제에 실패했습니다."
-}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -518,21 +509,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  "id" : 1
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>성공시(201)
-응답 데이터 없음
-실패시(400)
-{ 
-  "errorMessage" : "수정에 실패했습니다."
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>성공시(200)
 {
     "regDt": "2023-06-07T20:57:33.267995",
@@ -560,11 +536,45 @@
     <t>/api/board/update/{게시글번호}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>성공시(200)
+응답 데이터 없음
+실패시(400)
+{
+  "status" : "Bad_Request", 
+  "errorMessage" : "삭제에 실패했습니다."
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST / application/json</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "subject" : "(수정)글제목",
+  "content" : "(수정)글내용"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공시(201)
+응답 데이터 없음
+실패시(400)
+{ 
+  "errorMessage" : "등록되지 않은 게시글 입니다."
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1315,8 +1325,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1339,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -1356,22 +1366,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1381,16 +1391,16 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1400,16 +1410,16 @@
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -1419,16 +1429,16 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -1438,16 +1448,16 @@
       <c r="B6" s="19"/>
       <c r="C6" s="18"/>
       <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -1586,13 +1596,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -1602,7 +1612,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1663,7 +1673,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
@@ -1691,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -1728,10 +1738,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>14</v>
@@ -1748,19 +1758,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1800,7 +1810,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -1843,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1855,13 +1865,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -1871,7 +1881,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1975,16 +1985,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>9</v>
@@ -1995,19 +2005,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2015,19 +2025,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2035,19 +2045,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2055,19 +2065,19 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2075,19 +2085,19 @@
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.15">
@@ -2095,7 +2105,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -2138,7 +2148,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2150,13 +2160,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2166,7 +2176,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2290,19 +2300,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2313,7 +2323,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>14</v>
@@ -2333,7 +2343,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>14</v>
@@ -2366,7 +2376,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -2388,6 +2398,241 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B20:F20"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2409,7 +2654,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2421,13 +2666,13 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -2437,7 +2682,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -2470,53 +2715,63 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -2613,242 +2868,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B20:F20"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>

</xml_diff>